<commit_message>
move map with player
</commit_message>
<xml_diff>
--- a/Resources/gamedata/units.xlsx
+++ b/Resources/gamedata/units.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>name</t>
   </si>
@@ -24,10 +24,13 @@
     <t>id</t>
   </si>
   <si>
-    <t>speedx</t>
+    <t>speed</t>
   </si>
   <si>
-    <t>speedy</t>
+    <t>score</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -360,16 +363,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -382,6 +385,9 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>